<commit_message>
Correct Data and insert.py
</commit_message>
<xml_diff>
--- a/Phase2-Project Design document/data/customer.xlsx
+++ b/Phase2-Project Design document/data/customer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>Jayanth</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>pswd</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Satwik</t>
+  </si>
+  <si>
+    <t>Heemmanshu</t>
   </si>
 </sst>
 </file>
@@ -941,13 +956,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,8 +974,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -968,8 +991,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -979,8 +1008,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -990,8 +1025,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1001,8 +1042,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1012,8 +1059,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1023,8 +1076,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1034,8 +1093,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1045,8 +1110,14 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1056,8 +1127,14 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1067,8 +1144,14 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1078,8 +1161,14 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1089,8 +1178,14 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1100,8 +1195,14 @@
       <c r="C14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1111,8 +1212,14 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1122,8 +1229,14 @@
       <c r="C16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1133,8 +1246,14 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1144,8 +1263,14 @@
       <c r="C18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1155,8 +1280,14 @@
       <c r="C19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1166,8 +1297,14 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1176,6 +1313,12 @@
       </c>
       <c r="C21" t="s">
         <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>